<commit_message>
Update regresi web testing
</commit_message>
<xml_diff>
--- a/Data Test/contact_us.xlsx
+++ b/Data Test/contact_us.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\1. UNNES\6. Semester 6\2 - MSIB\CAPSTONE PROJECT\testing-lms\Data Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79CE8936-EF71-4062-94A0-8BE47AB247CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DFE6A44-32CA-4122-8F8A-B32B499E7944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4995" yWindow="4305" windowWidth="18000" windowHeight="9270" xr2:uid="{45076FA3-564A-4E50-94CC-5AE5A21FCC3F}"/>
+    <workbookView xWindow="2235" yWindow="1590" windowWidth="18000" windowHeight="9270" xr2:uid="{45076FA3-564A-4E50-94CC-5AE5A21FCC3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,16 +65,16 @@
     <t>TC003</t>
   </si>
   <si>
-    <t>salgmail.com</t>
-  </si>
-  <si>
-    <t>sal</t>
-  </si>
-  <si>
-    <t>sal@gmail.com</t>
-  </si>
-  <si>
-    <t>Hi.</t>
+    <t>Archen Aydin</t>
+  </si>
+  <si>
+    <t>archen</t>
+  </si>
+  <si>
+    <t>archen@gmail.com</t>
+  </si>
+  <si>
+    <t>I have problem to sign in with my account, archen@gmail.com is the email that I use for the account, please help me to fix it.</t>
   </si>
 </sst>
 </file>
@@ -148,12 +148,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -472,15 +483,15 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="1" max="2" width="10.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" style="5" customWidth="1"/>
     <col min="6" max="6" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -494,55 +505,55 @@
       <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>